<commit_message>
halved space usage of reverse list
</commit_message>
<xml_diff>
--- a/spreadsheets/challenge1_space_usage.xlsx
+++ b/spreadsheets/challenge1_space_usage.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/al/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/al/repos/metric_space/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9555F1-71EF-B64B-ACC9-C46E281EC187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905D472A-BC7C-D740-8E3B-7FCCE204CC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20600" yWindow="500" windowWidth="30380" windowHeight="19560" xr2:uid="{E1B58356-ABED-684B-92EB-3EB3B0EDAAA4}"/>
+    <workbookView xWindow="140" yWindow="500" windowWidth="30380" windowHeight="19560" xr2:uid="{E1B58356-ABED-684B-92EB-3EB3B0EDAAA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>dims</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>per item</t>
+  </si>
+  <si>
+    <t>EVP&lt;2&gt;</t>
+  </si>
+  <si>
+    <t>Naility</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>usize</t>
   </si>
 </sst>
 </file>
@@ -485,63 +497,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F8336C-9234-A840-A0BF-6C824A0F59AF}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D1" s="1">
         <v>27000000</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>384</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D6" t="s">
+    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
       </c>
       <c r="G6" t="s">
         <v>16</v>
@@ -552,252 +563,273 @@
       <c r="I6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>22</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>2</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>3</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>4</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1">
-        <f>C1</f>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1">
+        <f>D1</f>
         <v>27000000</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>1</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1024</v>
       </c>
-      <c r="E9">
-        <f>D9/8</f>
+      <c r="F9">
+        <f>E9/8</f>
         <v>128</v>
       </c>
-      <c r="F9" s="1">
-        <f>B9*C9*E9</f>
+      <c r="G9" s="1">
+        <f>C9*D9*F9</f>
         <v>3456000000</v>
       </c>
-      <c r="G9" s="1">
-        <f>F9/1024</f>
+      <c r="H9" s="1">
+        <f t="shared" ref="H9:J14" si="0">G9/1024</f>
         <v>3375000</v>
       </c>
-      <c r="H9" s="1">
-        <f>G9/1024</f>
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
         <v>3295.8984375</v>
       </c>
-      <c r="I9" s="1">
-        <f>H9/1024</f>
+      <c r="J9" s="1">
+        <f t="shared" si="0"/>
         <v>3.2186508178710938</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1">
-        <f>C1</f>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1">
+        <f>D1</f>
         <v>27000000</v>
       </c>
-      <c r="C10">
-        <f>C3</f>
+      <c r="D10">
+        <f>D3</f>
         <v>6</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>64</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>8</v>
       </c>
-      <c r="F10" s="1">
-        <f t="shared" ref="F10:F14" si="0">B10*C10*E10</f>
+      <c r="G10" s="1">
+        <f t="shared" ref="G10:G14" si="1">C10*D10*F10</f>
         <v>1296000000</v>
       </c>
-      <c r="G10" s="1">
-        <f>F10/1024</f>
+      <c r="H10" s="1">
+        <f t="shared" si="0"/>
         <v>1265625</v>
       </c>
-      <c r="H10" s="1">
-        <f>G10/1024</f>
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
         <v>1235.9619140625</v>
       </c>
-      <c r="I10" s="1">
-        <f>H10/1024</f>
+      <c r="J10" s="1">
+        <f t="shared" si="0"/>
         <v>1.2069940567016602</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
-        <f>C1</f>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1">
+        <f>D1</f>
         <v>27000000</v>
       </c>
-      <c r="C11">
-        <f>C3</f>
+      <c r="D11">
+        <f>D3</f>
         <v>6</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>64</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>8</v>
       </c>
-      <c r="F11" s="1">
-        <f t="shared" si="0"/>
+      <c r="G11" s="1">
+        <f t="shared" si="1"/>
         <v>1296000000</v>
       </c>
-      <c r="G11">
-        <f>F11/1024</f>
+      <c r="H11">
+        <f t="shared" si="0"/>
         <v>1265625</v>
       </c>
-      <c r="H11">
-        <f>G11/1024</f>
+      <c r="I11">
+        <f t="shared" si="0"/>
         <v>1235.9619140625</v>
       </c>
-      <c r="I11">
-        <f>H11/1024</f>
+      <c r="J11">
+        <f t="shared" si="0"/>
         <v>1.2069940567016602</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
-        <f>C1</f>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1">
+        <f>D1</f>
         <v>27000000</v>
       </c>
-      <c r="C12">
-        <f>C3</f>
+      <c r="D12">
+        <f>D3</f>
         <v>6</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1024</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>8</v>
       </c>
-      <c r="F12" s="1">
-        <f t="shared" si="0"/>
+      <c r="G12" s="1">
+        <f t="shared" si="1"/>
         <v>1296000000</v>
       </c>
-      <c r="G12">
-        <f>F12/1024</f>
+      <c r="H12">
+        <f t="shared" si="0"/>
         <v>1265625</v>
       </c>
-      <c r="H12">
-        <f>G12/1024</f>
+      <c r="I12">
+        <f t="shared" si="0"/>
         <v>1235.9619140625</v>
       </c>
-      <c r="I12">
-        <f>H12/1024</f>
+      <c r="J12">
+        <f t="shared" si="0"/>
         <v>1.2069940567016602</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1">
-        <f>B12</f>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1">
+        <f>C12</f>
         <v>27000000</v>
       </c>
-      <c r="C13">
-        <f>C3</f>
+      <c r="D13">
+        <f>D3</f>
         <v>6</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>1024</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>8</v>
       </c>
-      <c r="F13" s="1">
-        <f t="shared" si="0"/>
+      <c r="G13" s="1">
+        <f t="shared" si="1"/>
         <v>1296000000</v>
       </c>
-      <c r="G13">
-        <f>F13/1024</f>
+      <c r="H13">
+        <f t="shared" si="0"/>
         <v>1265625</v>
       </c>
-      <c r="H13">
-        <f>G13/1024</f>
+      <c r="I13">
+        <f t="shared" si="0"/>
         <v>1235.9619140625</v>
       </c>
-      <c r="I13">
-        <f>H13/1024</f>
+      <c r="J13">
+        <f t="shared" si="0"/>
         <v>1.2069940567016602</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
-        <f>B13</f>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="1">
+        <f>C13</f>
         <v>27000000</v>
       </c>
-      <c r="C14">
-        <f>C4</f>
+      <c r="D14">
+        <f>D4</f>
         <v>10</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E14" s="2">
         <v>64</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>8</v>
       </c>
-      <c r="F14" s="1">
-        <f t="shared" si="0"/>
+      <c r="G14" s="1">
+        <f t="shared" si="1"/>
         <v>2160000000</v>
       </c>
-      <c r="G14">
-        <f>F14/1024</f>
+      <c r="H14">
+        <f t="shared" si="0"/>
         <v>2109375</v>
       </c>
-      <c r="H14">
-        <f>G14/1024</f>
+      <c r="I14">
+        <f t="shared" si="0"/>
         <v>2059.9365234375</v>
       </c>
-      <c r="I14">
-        <f>H14/1024</f>
+      <c r="J14">
+        <f t="shared" si="0"/>
         <v>2.0116567611694336</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G16" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="1">
-        <f>SUM(I9:I14)</f>
+      <c r="J16" s="1">
+        <f>SUM(J9:J14)</f>
         <v>10.058283805847168</v>
       </c>
     </row>

</xml_diff>